<commit_message>
[CAN2-22] Ready for Review as per [CAN2-29]
[CAN2-22] Requirements are ready for a review by @boomshakakan as per [CAN2-29].
</commit_message>
<xml_diff>
--- a/CAN_Controller_Design_Specifications_Andrew.xlsx
+++ b/CAN_Controller_Design_Specifications_Andrew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE2F3D-9643-49E7-A371-60C4453A644F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8046AE-905B-437F-81D0-7DE88005E9A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="311">
   <si>
     <t>Requirement Header</t>
   </si>
@@ -944,6 +944,21 @@
   </si>
   <si>
     <t>The Module shall set int_txframe_reg[((i_send_data[67:64]+1)*4 + 51):((i_send_data[67:64]+1)*4 + 61)] equal to 11'b10111111111 when int_mstate is LOOPBACK, int_tstate is BUSY and i_send_data[108] is logic high.</t>
+  </si>
+  <si>
+    <t>Frame Reception</t>
+  </si>
+  <si>
+    <t>BSP_SOVR_05</t>
+  </si>
+  <si>
+    <t>BSP_SOVR_06</t>
+  </si>
+  <si>
+    <t>The Module shall set int_tx_send_bit equal to logic high when i_samp_tick is logic high and int_tstate is either IFS or IDLE.</t>
+  </si>
+  <si>
+    <t>The Module shall set o_tx_bit equal to logic high when i_samp_tick is logic high and int_tstate is either IFS or IDLE.</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1000,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1306,21 +1321,10 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1328,7 +1332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1343,14 +1347,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,54 +1404,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1692,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A146"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,1493 +1719,1503 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="13" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="13" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="14" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="13" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="13" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="14" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="13" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="14" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="9"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="13" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="14" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="13" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
+      <c r="A25" s="42"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="42"/>
+      <c r="B26" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="11" t="s">
+      <c r="A27" s="42"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="11" t="s">
+      <c r="A29" s="42"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="11" t="s">
+      <c r="A31" s="42"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="11" t="s">
+      <c r="A33" s="42"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="11" t="s">
+      <c r="A35" s="42"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="13"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="11" t="s">
+      <c r="A37" s="42"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="11" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="11" t="s">
+      <c r="A41" s="42"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="11" t="s">
+      <c r="A43" s="42"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="11" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="11" t="s">
+      <c r="A47" s="42"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="44"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="16" t="s">
+      <c r="A49" s="42"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="12" t="s">
+      <c r="A50" s="42"/>
+      <c r="B50" s="38" t="s">
         <v>78</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="11" t="s">
+      <c r="A51" s="42"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="13"/>
+      <c r="A52" s="42"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="11" t="s">
+      <c r="A53" s="42"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="44"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15" t="s">
+      <c r="A54" s="42"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="19" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="27" t="s">
+      <c r="A55" s="42"/>
+      <c r="B55" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
+      <c r="A56" s="42"/>
       <c r="B56" s="30"/>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="18" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
+      <c r="A57" s="42"/>
       <c r="B57" s="30"/>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="13" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
+      <c r="A58" s="42"/>
       <c r="B58" s="30"/>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D58" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="44"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="16" t="s">
+      <c r="A59" s="42"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="16" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="27" t="s">
+      <c r="A60" s="42"/>
+      <c r="B60" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="24" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="42"/>
       <c r="B61" s="30"/>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="13" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
+      <c r="A62" s="42"/>
       <c r="B62" s="30"/>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D62" s="18" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="44"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="16" t="s">
+      <c r="A63" s="42"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D63" s="16" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="27" t="s">
+      <c r="A64" s="42"/>
+      <c r="B64" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
+      <c r="A65" s="42"/>
       <c r="B65" s="30"/>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="13" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
+      <c r="A66" s="42"/>
       <c r="B66" s="30"/>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="D66" s="24" t="s">
+      <c r="D66" s="18" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
+      <c r="A67" s="42"/>
       <c r="B67" s="30"/>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D67" s="13" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="42"/>
       <c r="B68" s="30"/>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="18" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
+      <c r="A69" s="42"/>
       <c r="B69" s="30"/>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="13" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
+      <c r="A70" s="42"/>
       <c r="B70" s="30"/>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="D70" s="24" t="s">
+      <c r="D70" s="18" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
+      <c r="A71" s="42"/>
       <c r="B71" s="30"/>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D71" s="13" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
+      <c r="A72" s="42"/>
       <c r="B72" s="30"/>
-      <c r="C72" s="26" t="s">
+      <c r="C72" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D72" s="18" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="44"/>
+      <c r="A73" s="42"/>
       <c r="B73" s="30"/>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="D73" s="13" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="42"/>
       <c r="B74" s="30"/>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="24" t="s">
+      <c r="D74" s="18" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
+      <c r="A75" s="42"/>
       <c r="B75" s="30"/>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D75" s="13" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
+      <c r="A76" s="42"/>
       <c r="B76" s="30"/>
-      <c r="C76" s="26" t="s">
+      <c r="C76" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D76" s="24" t="s">
+      <c r="D76" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
+      <c r="A77" s="42"/>
       <c r="B77" s="30"/>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="13" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="44"/>
+      <c r="A78" s="42"/>
       <c r="B78" s="30"/>
-      <c r="C78" s="26" t="s">
+      <c r="C78" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D78" s="24" t="s">
+      <c r="D78" s="18" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
+      <c r="A79" s="42"/>
       <c r="B79" s="30"/>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="42"/>
       <c r="B80" s="30"/>
-      <c r="C80" s="26" t="s">
+      <c r="C80" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="D80" s="24" t="s">
+      <c r="D80" s="18" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="44"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="11" t="s">
+      <c r="A81" s="42"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="D81" s="16" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
-      <c r="B82" s="36" t="s">
+      <c r="A82" s="42"/>
+      <c r="B82" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D82" s="24" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="11" t="s">
+      <c r="A83" s="42"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D83" s="19" t="s">
+      <c r="D83" s="13" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="26" t="s">
+      <c r="A84" s="42"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="D84" s="24" t="s">
+      <c r="D84" s="18" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="11" t="s">
+      <c r="A85" s="42"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="D85" s="13" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="26" t="s">
+      <c r="A86" s="42"/>
+      <c r="B86" s="33"/>
+      <c r="C86" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="24" t="s">
+      <c r="D86" s="18" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="11" t="s">
+      <c r="A87" s="42"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="13" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="26" t="s">
+      <c r="A88" s="42"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="D88" s="24" t="s">
+      <c r="D88" s="18" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="11" t="s">
+      <c r="A89" s="42"/>
+      <c r="B89" s="33"/>
+      <c r="C89" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="13" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="44"/>
-      <c r="B90" s="40"/>
-      <c r="C90" s="34" t="s">
+      <c r="A90" s="42"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="D90" s="35" t="s">
+      <c r="D90" s="26" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
-      <c r="B91" s="36" t="s">
+      <c r="A91" s="42"/>
+      <c r="B91" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C91" s="28" t="s">
+      <c r="C91" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="22" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="26" t="s">
+      <c r="A92" s="42"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="D92" s="24" t="s">
+      <c r="D92" s="18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="11" t="s">
+      <c r="A93" s="42"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D93" s="13" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="26" t="s">
+      <c r="A94" s="42"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="D94" s="24" t="s">
+      <c r="D94" s="18" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="11" t="s">
+      <c r="A95" s="42"/>
+      <c r="B95" s="33"/>
+      <c r="C95" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D95" s="19" t="s">
+      <c r="D95" s="13" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="26" t="s">
+      <c r="A96" s="42"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="D96" s="24" t="s">
+      <c r="D96" s="18" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="11" t="s">
+      <c r="A97" s="42"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D97" s="19" t="s">
+      <c r="D97" s="13" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="26" t="s">
+      <c r="A98" s="42"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D98" s="24" t="s">
+      <c r="D98" s="18" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="44"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="11" t="s">
+      <c r="A99" s="42"/>
+      <c r="B99" s="33"/>
+      <c r="C99" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D99" s="19" t="s">
+      <c r="D99" s="13" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
-      <c r="B100" s="37"/>
-      <c r="C100" s="26" t="s">
+      <c r="A100" s="42"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D100" s="24" t="s">
+      <c r="D100" s="18" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="44"/>
-      <c r="B101" s="37"/>
-      <c r="C101" s="16" t="s">
+      <c r="A101" s="42"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D101" s="22" t="s">
+      <c r="D101" s="16" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
-      <c r="B102" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C102" s="32" t="s">
+      <c r="A102" s="42"/>
+      <c r="B102" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="C102" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D102" s="33" t="s">
+      <c r="D102" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="44"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="16" t="s">
+      <c r="A103" s="42"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="D103" s="22" t="s">
+      <c r="D103" s="16" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="44"/>
-      <c r="B104" s="27" t="s">
+      <c r="A104" s="42"/>
+      <c r="B104" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="C104" s="32" t="s">
+      <c r="C104" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="D104" s="33" t="s">
+      <c r="D104" s="24" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="44"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="16" t="s">
+      <c r="A105" s="42"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D105" s="22" t="s">
+      <c r="D105" s="16" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="44"/>
-      <c r="B106" s="27" t="s">
+      <c r="A106" s="42"/>
+      <c r="B106" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="C106" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="D106" s="33" t="s">
+      <c r="D106" s="24" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="44"/>
+      <c r="A107" s="42"/>
       <c r="B107" s="30"/>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D107" s="19" t="s">
+      <c r="D107" s="13" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
+      <c r="A108" s="42"/>
       <c r="B108" s="30"/>
-      <c r="C108" s="26" t="s">
+      <c r="C108" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="D108" s="24" t="s">
+      <c r="D108" s="18" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="44"/>
+      <c r="A109" s="42"/>
       <c r="B109" s="30"/>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="13" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="44"/>
+      <c r="A110" s="42"/>
       <c r="B110" s="30"/>
-      <c r="C110" s="26" t="s">
+      <c r="C110" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="D110" s="24" t="s">
+      <c r="D110" s="18" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="44"/>
+      <c r="A111" s="42"/>
       <c r="B111" s="30"/>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D111" s="19" t="s">
+      <c r="D111" s="13" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="42"/>
       <c r="B112" s="30"/>
-      <c r="C112" s="26" t="s">
+      <c r="C112" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="D112" s="24" t="s">
+      <c r="D112" s="18" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="44"/>
+      <c r="A113" s="42"/>
       <c r="B113" s="30"/>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="D113" s="19" t="s">
+      <c r="D113" s="13" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="42"/>
       <c r="B114" s="30"/>
-      <c r="C114" s="26" t="s">
+      <c r="C114" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="D114" s="24" t="s">
+      <c r="D114" s="18" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="44"/>
+      <c r="A115" s="42"/>
       <c r="B115" s="30"/>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="D115" s="19" t="s">
+      <c r="D115" s="13" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="44"/>
+      <c r="A116" s="42"/>
       <c r="B116" s="30"/>
-      <c r="C116" s="26" t="s">
+      <c r="C116" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="D116" s="24" t="s">
+      <c r="D116" s="18" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="44"/>
+      <c r="A117" s="42"/>
       <c r="B117" s="30"/>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="13" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="44"/>
+      <c r="A118" s="42"/>
       <c r="B118" s="30"/>
-      <c r="C118" s="26" t="s">
+      <c r="C118" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="D118" s="24" t="s">
+      <c r="D118" s="18" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="44"/>
+      <c r="A119" s="42"/>
       <c r="B119" s="30"/>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="D119" s="19" t="s">
+      <c r="D119" s="13" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="44"/>
+      <c r="A120" s="42"/>
       <c r="B120" s="30"/>
-      <c r="C120" s="26" t="s">
+      <c r="C120" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="D120" s="24" t="s">
+      <c r="D120" s="18" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="44"/>
+      <c r="A121" s="42"/>
       <c r="B121" s="30"/>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D121" s="19" t="s">
+      <c r="D121" s="13" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="44"/>
+      <c r="A122" s="42"/>
       <c r="B122" s="30"/>
-      <c r="C122" s="26" t="s">
+      <c r="C122" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="D122" s="24" t="s">
+      <c r="D122" s="18" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="44"/>
+      <c r="A123" s="42"/>
       <c r="B123" s="30"/>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D123" s="19" t="s">
+      <c r="D123" s="13" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="44"/>
+      <c r="A124" s="42"/>
       <c r="B124" s="30"/>
-      <c r="C124" s="26" t="s">
+      <c r="C124" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="D124" s="24" t="s">
+      <c r="D124" s="18" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="44"/>
+      <c r="A125" s="42"/>
       <c r="B125" s="30"/>
-      <c r="C125" s="11" t="s">
+      <c r="C125" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="D125" s="19" t="s">
+      <c r="D125" s="13" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="44"/>
+      <c r="A126" s="42"/>
       <c r="B126" s="30"/>
-      <c r="C126" s="26" t="s">
+      <c r="C126" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="D126" s="24" t="s">
+      <c r="D126" s="18" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="44"/>
+      <c r="A127" s="42"/>
       <c r="B127" s="30"/>
-      <c r="C127" s="11" t="s">
+      <c r="C127" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="D127" s="19" t="s">
+      <c r="D127" s="13" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="44"/>
+      <c r="A128" s="42"/>
       <c r="B128" s="30"/>
-      <c r="C128" s="26" t="s">
+      <c r="C128" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="D128" s="24" t="s">
+      <c r="D128" s="18" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="44"/>
+      <c r="A129" s="42"/>
       <c r="B129" s="30"/>
-      <c r="C129" s="11" t="s">
+      <c r="C129" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="D129" s="19" t="s">
+      <c r="D129" s="13" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="44"/>
+      <c r="A130" s="42"/>
       <c r="B130" s="30"/>
-      <c r="C130" s="26" t="s">
+      <c r="C130" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="D130" s="24" t="s">
+      <c r="D130" s="18" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="44"/>
+      <c r="A131" s="42"/>
       <c r="B131" s="30"/>
-      <c r="C131" s="11" t="s">
+      <c r="C131" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="D131" s="19" t="s">
+      <c r="D131" s="13" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="44"/>
+      <c r="A132" s="42"/>
       <c r="B132" s="30"/>
-      <c r="C132" s="26" t="s">
+      <c r="C132" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="D132" s="24" t="s">
+      <c r="D132" s="18" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="44"/>
+      <c r="A133" s="42"/>
       <c r="B133" s="30"/>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D133" s="19" t="s">
+      <c r="D133" s="13" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="44"/>
+      <c r="A134" s="42"/>
       <c r="B134" s="30"/>
-      <c r="C134" s="26" t="s">
+      <c r="C134" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="D134" s="24" t="s">
+      <c r="D134" s="18" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="44"/>
+      <c r="A135" s="42"/>
       <c r="B135" s="30"/>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="D135" s="19" t="s">
+      <c r="D135" s="13" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="44"/>
+      <c r="A136" s="42"/>
       <c r="B136" s="30"/>
-      <c r="C136" s="26" t="s">
+      <c r="C136" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="D136" s="24" t="s">
+      <c r="D136" s="18" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="44"/>
+      <c r="A137" s="42"/>
       <c r="B137" s="30"/>
-      <c r="C137" s="11" t="s">
+      <c r="C137" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D137" s="19" t="s">
+      <c r="D137" s="13" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="44"/>
+      <c r="A138" s="42"/>
       <c r="B138" s="30"/>
-      <c r="C138" s="26" t="s">
+      <c r="C138" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="D138" s="24" t="s">
+      <c r="D138" s="18" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="44"/>
+      <c r="A139" s="42"/>
       <c r="B139" s="30"/>
-      <c r="C139" s="11" t="s">
+      <c r="C139" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D139" s="19" t="s">
+      <c r="D139" s="13" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="44"/>
+      <c r="A140" s="42"/>
       <c r="B140" s="30"/>
-      <c r="C140" s="26" t="s">
+      <c r="C140" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="D140" s="24" t="s">
+      <c r="D140" s="18" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="44"/>
+      <c r="A141" s="42"/>
       <c r="B141" s="30"/>
-      <c r="C141" s="11" t="s">
+      <c r="C141" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="D141" s="19" t="s">
+      <c r="D141" s="13" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="44"/>
-      <c r="B142" s="38"/>
-      <c r="C142" s="41" t="s">
+      <c r="A142" s="42"/>
+      <c r="B142" s="35"/>
+      <c r="C142" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="D142" s="39" t="s">
+      <c r="D142" s="27" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="44"/>
-      <c r="B143" s="27" t="s">
+      <c r="A143" s="42"/>
+      <c r="B143" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="C143" s="28" t="s">
+      <c r="C143" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="D143" s="29" t="s">
+      <c r="D143" s="22" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="44"/>
+      <c r="A144" s="42"/>
       <c r="B144" s="30"/>
-      <c r="C144" s="26" t="s">
+      <c r="C144" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="D144" s="24" t="s">
+      <c r="D144" s="18" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="44"/>
+      <c r="A145" s="42"/>
       <c r="B145" s="30"/>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="D145" s="19" t="s">
+      <c r="D145" s="13" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="44"/>
-      <c r="B146" s="31"/>
-      <c r="C146" s="34" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="42"/>
+      <c r="B146" s="30"/>
+      <c r="C146" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="D146" s="35" t="s">
+      <c r="D146" s="18" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="42"/>
-      <c r="C147" s="17"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="42"/>
-      <c r="C148" s="17"/>
+      <c r="A147" s="42"/>
+      <c r="B147" s="30"/>
+      <c r="C147" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D147" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="42"/>
+      <c r="B148" s="31"/>
+      <c r="C148" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="D148" s="26" t="s">
+        <v>310</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B143:B146"/>
-    <mergeCell ref="A2:A146"/>
     <mergeCell ref="B91:B101"/>
     <mergeCell ref="B82:B90"/>
     <mergeCell ref="B102:B103"/>
@@ -3217,6 +3227,8 @@
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="B50:B54"/>
     <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B143:B148"/>
+    <mergeCell ref="A2:A148"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CAN2-23] Ready for Review [CAN2-30]
[CAN2-23] Ready for Review by @colinfritzltts  as per [CAN2-30].
</commit_message>
<xml_diff>
--- a/CAN_Controller_Design_Specifications_Andrew.xlsx
+++ b/CAN_Controller_Design_Specifications_Andrew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8046AE-905B-437F-81D0-7DE88005E9A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AACD61E-9B5E-4877-904A-B0A61BCE4D82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bit Stream Processor" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="388">
   <si>
     <t>Requirement Header</t>
   </si>
@@ -959,6 +959,237 @@
   </si>
   <si>
     <t>The Module shall set o_tx_bit equal to logic high when i_samp_tick is logic high and int_tstate is either IFS or IDLE.</t>
+  </si>
+  <si>
+    <t>BTM</t>
+  </si>
+  <si>
+    <t>BTM_INIT_01</t>
+  </si>
+  <si>
+    <t>BTM_RST_01</t>
+  </si>
+  <si>
+    <t>The Module shall initialize o_samp_tick to logic low on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize o_rx_bit to logic high on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize can_phy_tx to logic high on system startup.</t>
+  </si>
+  <si>
+    <t>BTM_INIT_02</t>
+  </si>
+  <si>
+    <t>BTM_INIT_03</t>
+  </si>
+  <si>
+    <t>BTM_RST_02</t>
+  </si>
+  <si>
+    <t>BTM_RST_03</t>
+  </si>
+  <si>
+    <t>The Module shall initialize o_samp_tick to logic low when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize can_phy_tx to logic high when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize o_rx_bit to logic high when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>FSM</t>
+  </si>
+  <si>
+    <t>BTM_FSM_01</t>
+  </si>
+  <si>
+    <t>The Module shall set int_state equal to the int_state_next on rising edge of can_clk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Module shall set int_state_counter to int_state_counter + 1 on rising edge of can_clk. </t>
+  </si>
+  <si>
+    <t>BTM_FSM_02</t>
+  </si>
+  <si>
+    <t>BTM_FSM_03</t>
+  </si>
+  <si>
+    <t>BTM_FSM_04</t>
+  </si>
+  <si>
+    <t>BTM_FSM_05</t>
+  </si>
+  <si>
+    <t>BTM_FSM_06</t>
+  </si>
+  <si>
+    <t>The Module shall set int_state_counter to 0 when int_state is SYNC.</t>
+  </si>
+  <si>
+    <t>Syncronization</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_01</t>
+  </si>
+  <si>
+    <t>The Module shall set int_samp_tick equal to logic high when int_state is TS1 and int_state_next is TS2.</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_02</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_03</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_04</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_05</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_06</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_07</t>
+  </si>
+  <si>
+    <t>The Module shall set o_samp_tick equal to int_samp_tick on a rising edge of can_clk.</t>
+  </si>
+  <si>
+    <t>The Module shall set can_phy_tx equal to i_tx_bit when int_state is SYNC.</t>
+  </si>
+  <si>
+    <t>The Module shall hold the value of can_phy_tx when int_state is either TS1 or TS2.</t>
+  </si>
+  <si>
+    <t>BTM_RST_04</t>
+  </si>
+  <si>
+    <t>BTM_RST_05</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_state to SYNC when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_state_next to SYNC when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>BTM_INIT_04</t>
+  </si>
+  <si>
+    <t>BTM_INIT_05</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_state_next to SYNC on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_state to SYNC on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall set o_rx_bit equal to can_phy_rx when int_samp_tick is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall hold the value of o_rx_bit when int_samp_tick is logic low.</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_08</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rx_compare equal to can_phy_rx on a rising edge of can_clk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Module shall set int_state_next to SYNC when int_state_counter is greater than or equal to int_ts1 + int_ts2. </t>
+  </si>
+  <si>
+    <t>BTM_INIT_06</t>
+  </si>
+  <si>
+    <t>BTM_INIT_07</t>
+  </si>
+  <si>
+    <t>BTM_RST_06</t>
+  </si>
+  <si>
+    <t>BTM_RST_07</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_09</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_10</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_11</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_12</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_13</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_14</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_15</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rx_prev_compare equal to int_rx_compare on a rising edge of can_clk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Module shall set int_state_next to TS1 when int_state is either SYNC or PROP and int_state_counter is less than int_ts1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Module shall set int_state_next to TS2 when int_state_counter is less than int_ts1 + int_ts2. </t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts2 equal to i_ts2 + 1 on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts1 equal to i_ts1 + 1 on system startup.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts2 equal to i_ts2 + 1 when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts1 equal to i_ts1 + 1 when i_reset is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_ts2  to int_ts2 - i_sjw when int_rx_prev_compare is not equal to int_rx_compare, and int_state_counter is less than int_ts1 - i_sjw.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_ts2  to int_ts2 - int_state_counter when int_rx_prev_compare is not equal to int_rx_compare, int_state_counter is less than int_ts1, and int_state_counter is greater than or equal to int_ts1 - i_sjw.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts2 equal to i_ts2 + 1 when int_state is SYNC and int_rxbit_history[5:0] is either 6'b000000 or 6'b111111.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts1 equal to i_ts1 + 1 when int_state is SYNC and int_rxbit_history[5:0] is either 6'b000000 or 6'b111111.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts1 equal to int_ts1_next when int_state is SYNC and int_rxbit_history[5:0] is neither 6'b000000 or 6'b111111.</t>
+  </si>
+  <si>
+    <t>The Module shall initialize int_ts2 equal to int_ts2_next when int_state is SYNC and int_rxbit_history[5:0] is neither 6'b000000 or 6'b111111.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rxbit_history[5:0] to int_rxbit_history[4:0]&amp;can_phy_rx when int_state is SYNC.</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_16</t>
+  </si>
+  <si>
+    <t>BTM_SYNC_17</t>
+  </si>
+  <si>
+    <t>The Module shall set int_ts1_next to int_state_counter when int_rx_prev_compare is not equal to int_rx_compare, int_state_counter is greater than or equal int_ts1, and int_state_counter is less than int_ts1 + i_sjw.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_ts1_next  to int_ts1+ i_sjw when int_rx_prev_compare is not equal to int_rx_compare, and int_state_counter is less than int_ts1 + i_sjw.</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1328,11 +1559,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1368,15 +1636,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,7 +1645,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1404,12 +1669,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1692,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +2013,7 @@
       <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -1734,7 +2025,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
-      <c r="B3" s="37"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1744,7 +2035,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
-      <c r="B4" s="37"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +2045,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
-      <c r="B5" s="37"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1764,7 +2055,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="42"/>
-      <c r="B6" s="37"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +2065,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
-      <c r="B7" s="37"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1784,7 +2075,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
-      <c r="B8" s="37"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1794,7 +2085,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
-      <c r="B9" s="37"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +2095,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
-      <c r="B10" s="37"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1814,7 +2105,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
-      <c r="B11" s="37"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +2115,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
-      <c r="B12" s="37"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +2125,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
-      <c r="B13" s="37"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1844,7 +2135,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
-      <c r="B14" s="37"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1854,7 +2145,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
-      <c r="B15" s="37"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1864,7 +2155,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
-      <c r="B16" s="37"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1874,7 +2165,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
-      <c r="B17" s="37"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="7" t="s">
         <v>22</v>
       </c>
@@ -1884,7 +2175,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
-      <c r="B18" s="37"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1894,7 +2185,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
-      <c r="B19" s="37"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
       </c>
@@ -1904,7 +2195,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
-      <c r="B20" s="37"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1914,7 +2205,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
-      <c r="B21" s="37"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
@@ -1924,7 +2215,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="42"/>
-      <c r="B22" s="37"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +2225,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
-      <c r="B23" s="37"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="7" t="s">
         <v>28</v>
       </c>
@@ -1944,7 +2235,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
-      <c r="B24" s="37"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1954,7 +2245,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42"/>
-      <c r="B25" s="37"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1964,7 +2255,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1976,7 +2267,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
-      <c r="B27" s="39"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="9" t="s">
         <v>33</v>
       </c>
@@ -1986,7 +2277,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="42"/>
-      <c r="B28" s="39"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1996,7 +2287,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="42"/>
-      <c r="B29" s="39"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="9" t="s">
         <v>35</v>
       </c>
@@ -2006,7 +2297,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
-      <c r="B30" s="39"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2016,7 +2307,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
-      <c r="B31" s="39"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="9" t="s">
         <v>37</v>
       </c>
@@ -2026,7 +2317,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
-      <c r="B32" s="39"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2036,7 +2327,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
-      <c r="B33" s="39"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="9" t="s">
         <v>39</v>
       </c>
@@ -2046,7 +2337,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="42"/>
-      <c r="B34" s="39"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2056,7 +2347,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="42"/>
-      <c r="B35" s="39"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="9" t="s">
         <v>41</v>
       </c>
@@ -2066,7 +2357,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="42"/>
-      <c r="B36" s="39"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2076,7 +2367,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="42"/>
-      <c r="B37" s="39"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="9" t="s">
         <v>43</v>
       </c>
@@ -2086,7 +2377,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="42"/>
-      <c r="B38" s="39"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="1" t="s">
         <v>44</v>
       </c>
@@ -2096,7 +2387,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
-      <c r="B39" s="39"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
@@ -2106,7 +2397,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="42"/>
-      <c r="B40" s="39"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="1" t="s">
         <v>46</v>
       </c>
@@ -2116,7 +2407,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="42"/>
-      <c r="B41" s="39"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="9" t="s">
         <v>47</v>
       </c>
@@ -2126,7 +2417,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="42"/>
-      <c r="B42" s="39"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="1" t="s">
         <v>48</v>
       </c>
@@ -2136,7 +2427,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="42"/>
-      <c r="B43" s="39"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="9" t="s">
         <v>49</v>
       </c>
@@ -2146,7 +2437,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="42"/>
-      <c r="B44" s="39"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="1" t="s">
         <v>50</v>
       </c>
@@ -2156,7 +2447,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
-      <c r="B45" s="39"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="9" t="s">
         <v>51</v>
       </c>
@@ -2166,7 +2457,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="42"/>
-      <c r="B46" s="39"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="1" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2467,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="42"/>
-      <c r="B47" s="39"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="9" t="s">
         <v>53</v>
       </c>
@@ -2186,7 +2477,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="42"/>
-      <c r="B48" s="39"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2196,7 +2487,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="42"/>
-      <c r="B49" s="40"/>
+      <c r="B49" s="39"/>
       <c r="C49" s="11" t="s">
         <v>55</v>
       </c>
@@ -2206,7 +2497,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="42"/>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="37" t="s">
         <v>78</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -2218,7 +2509,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="42"/>
-      <c r="B51" s="39"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="9" t="s">
         <v>80</v>
       </c>
@@ -2228,7 +2519,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="42"/>
-      <c r="B52" s="39"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="1" t="s">
         <v>81</v>
       </c>
@@ -2238,7 +2529,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="42"/>
-      <c r="B53" s="39"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="9" t="s">
         <v>82</v>
       </c>
@@ -2248,7 +2539,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="42"/>
-      <c r="B54" s="40"/>
+      <c r="B54" s="39"/>
       <c r="C54" s="10" t="s">
         <v>83</v>
       </c>
@@ -2258,7 +2549,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="42"/>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="32" t="s">
         <v>92</v>
       </c>
       <c r="C55" s="21" t="s">
@@ -2270,7 +2561,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="42"/>
-      <c r="B56" s="30"/>
+      <c r="B56" s="34"/>
       <c r="C56" s="20" t="s">
         <v>95</v>
       </c>
@@ -2280,7 +2571,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="42"/>
-      <c r="B57" s="30"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="9" t="s">
         <v>96</v>
       </c>
@@ -2290,7 +2581,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="42"/>
-      <c r="B58" s="30"/>
+      <c r="B58" s="34"/>
       <c r="C58" s="20" t="s">
         <v>97</v>
       </c>
@@ -2300,7 +2591,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="42"/>
-      <c r="B59" s="35"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="11" t="s">
         <v>98</v>
       </c>
@@ -2310,7 +2601,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="42"/>
-      <c r="B60" s="29" t="s">
+      <c r="B60" s="32" t="s">
         <v>99</v>
       </c>
       <c r="C60" s="23" t="s">
@@ -2322,7 +2613,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="42"/>
-      <c r="B61" s="30"/>
+      <c r="B61" s="34"/>
       <c r="C61" s="9" t="s">
         <v>101</v>
       </c>
@@ -2332,7 +2623,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="42"/>
-      <c r="B62" s="30"/>
+      <c r="B62" s="34"/>
       <c r="C62" s="20" t="s">
         <v>102</v>
       </c>
@@ -2342,7 +2633,7 @@
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="42"/>
-      <c r="B63" s="35"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="11" t="s">
         <v>103</v>
       </c>
@@ -2352,7 +2643,7 @@
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="42"/>
-      <c r="B64" s="29" t="s">
+      <c r="B64" s="32" t="s">
         <v>146</v>
       </c>
       <c r="C64" s="23" t="s">
@@ -2364,7 +2655,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="42"/>
-      <c r="B65" s="30"/>
+      <c r="B65" s="34"/>
       <c r="C65" s="9" t="s">
         <v>148</v>
       </c>
@@ -2374,7 +2665,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="42"/>
-      <c r="B66" s="30"/>
+      <c r="B66" s="34"/>
       <c r="C66" s="20" t="s">
         <v>149</v>
       </c>
@@ -2384,7 +2675,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="42"/>
-      <c r="B67" s="30"/>
+      <c r="B67" s="34"/>
       <c r="C67" s="9" t="s">
         <v>150</v>
       </c>
@@ -2394,7 +2685,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="42"/>
-      <c r="B68" s="30"/>
+      <c r="B68" s="34"/>
       <c r="C68" s="20" t="s">
         <v>151</v>
       </c>
@@ -2404,7 +2695,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="42"/>
-      <c r="B69" s="30"/>
+      <c r="B69" s="34"/>
       <c r="C69" s="9" t="s">
         <v>152</v>
       </c>
@@ -2414,7 +2705,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="42"/>
-      <c r="B70" s="30"/>
+      <c r="B70" s="34"/>
       <c r="C70" s="20" t="s">
         <v>153</v>
       </c>
@@ -2424,7 +2715,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="42"/>
-      <c r="B71" s="30"/>
+      <c r="B71" s="34"/>
       <c r="C71" s="9" t="s">
         <v>154</v>
       </c>
@@ -2434,7 +2725,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="42"/>
-      <c r="B72" s="30"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="20" t="s">
         <v>155</v>
       </c>
@@ -2444,7 +2735,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="42"/>
-      <c r="B73" s="30"/>
+      <c r="B73" s="34"/>
       <c r="C73" s="9" t="s">
         <v>156</v>
       </c>
@@ -2454,7 +2745,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="42"/>
-      <c r="B74" s="30"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="20" t="s">
         <v>157</v>
       </c>
@@ -2464,7 +2755,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="42"/>
-      <c r="B75" s="30"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="9" t="s">
         <v>158</v>
       </c>
@@ -2474,7 +2765,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="42"/>
-      <c r="B76" s="30"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="20" t="s">
         <v>159</v>
       </c>
@@ -2484,7 +2775,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="42"/>
-      <c r="B77" s="30"/>
+      <c r="B77" s="34"/>
       <c r="C77" s="9" t="s">
         <v>160</v>
       </c>
@@ -2494,7 +2785,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="42"/>
-      <c r="B78" s="30"/>
+      <c r="B78" s="34"/>
       <c r="C78" s="20" t="s">
         <v>161</v>
       </c>
@@ -2504,7 +2795,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="42"/>
-      <c r="B79" s="30"/>
+      <c r="B79" s="34"/>
       <c r="C79" s="9" t="s">
         <v>162</v>
       </c>
@@ -2514,7 +2805,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="42"/>
-      <c r="B80" s="30"/>
+      <c r="B80" s="34"/>
       <c r="C80" s="20" t="s">
         <v>163</v>
       </c>
@@ -2524,7 +2815,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="42"/>
-      <c r="B81" s="35"/>
+      <c r="B81" s="33"/>
       <c r="C81" s="9" t="s">
         <v>164</v>
       </c>
@@ -2534,7 +2825,7 @@
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="42"/>
-      <c r="B82" s="32" t="s">
+      <c r="B82" s="29" t="s">
         <v>136</v>
       </c>
       <c r="C82" s="23" t="s">
@@ -2546,7 +2837,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="42"/>
-      <c r="B83" s="33"/>
+      <c r="B83" s="30"/>
       <c r="C83" s="9" t="s">
         <v>139</v>
       </c>
@@ -2556,7 +2847,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="42"/>
-      <c r="B84" s="33"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="20" t="s">
         <v>140</v>
       </c>
@@ -2566,7 +2857,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="42"/>
-      <c r="B85" s="33"/>
+      <c r="B85" s="30"/>
       <c r="C85" s="9" t="s">
         <v>141</v>
       </c>
@@ -2576,7 +2867,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="42"/>
-      <c r="B86" s="33"/>
+      <c r="B86" s="30"/>
       <c r="C86" s="20" t="s">
         <v>142</v>
       </c>
@@ -2586,7 +2877,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="42"/>
-      <c r="B87" s="33"/>
+      <c r="B87" s="30"/>
       <c r="C87" s="9" t="s">
         <v>143</v>
       </c>
@@ -2596,7 +2887,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="42"/>
-      <c r="B88" s="33"/>
+      <c r="B88" s="30"/>
       <c r="C88" s="20" t="s">
         <v>144</v>
       </c>
@@ -2606,7 +2897,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="42"/>
-      <c r="B89" s="33"/>
+      <c r="B89" s="30"/>
       <c r="C89" s="9" t="s">
         <v>145</v>
       </c>
@@ -2616,7 +2907,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="42"/>
-      <c r="B90" s="34"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="25" t="s">
         <v>212</v>
       </c>
@@ -2626,7 +2917,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="42"/>
-      <c r="B91" s="32" t="s">
+      <c r="B91" s="29" t="s">
         <v>165</v>
       </c>
       <c r="C91" s="21" t="s">
@@ -2638,7 +2929,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="42"/>
-      <c r="B92" s="33"/>
+      <c r="B92" s="30"/>
       <c r="C92" s="20" t="s">
         <v>168</v>
       </c>
@@ -2648,7 +2939,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="42"/>
-      <c r="B93" s="33"/>
+      <c r="B93" s="30"/>
       <c r="C93" s="9" t="s">
         <v>167</v>
       </c>
@@ -2658,7 +2949,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="42"/>
-      <c r="B94" s="33"/>
+      <c r="B94" s="30"/>
       <c r="C94" s="20" t="s">
         <v>169</v>
       </c>
@@ -2668,7 +2959,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="42"/>
-      <c r="B95" s="33"/>
+      <c r="B95" s="30"/>
       <c r="C95" s="9" t="s">
         <v>170</v>
       </c>
@@ -2678,7 +2969,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="42"/>
-      <c r="B96" s="33"/>
+      <c r="B96" s="30"/>
       <c r="C96" s="20" t="s">
         <v>171</v>
       </c>
@@ -2688,7 +2979,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="42"/>
-      <c r="B97" s="33"/>
+      <c r="B97" s="30"/>
       <c r="C97" s="9" t="s">
         <v>172</v>
       </c>
@@ -2698,7 +2989,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="42"/>
-      <c r="B98" s="33"/>
+      <c r="B98" s="30"/>
       <c r="C98" s="20" t="s">
         <v>173</v>
       </c>
@@ -2708,7 +2999,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="42"/>
-      <c r="B99" s="33"/>
+      <c r="B99" s="30"/>
       <c r="C99" s="9" t="s">
         <v>174</v>
       </c>
@@ -2718,7 +3009,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="42"/>
-      <c r="B100" s="33"/>
+      <c r="B100" s="30"/>
       <c r="C100" s="20" t="s">
         <v>175</v>
       </c>
@@ -2728,7 +3019,7 @@
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="42"/>
-      <c r="B101" s="33"/>
+      <c r="B101" s="30"/>
       <c r="C101" s="11" t="s">
         <v>176</v>
       </c>
@@ -2738,7 +3029,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="42"/>
-      <c r="B102" s="29" t="s">
+      <c r="B102" s="32" t="s">
         <v>306</v>
       </c>
       <c r="C102" s="23" t="s">
@@ -2750,7 +3041,7 @@
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="42"/>
-      <c r="B103" s="35"/>
+      <c r="B103" s="33"/>
       <c r="C103" s="11" t="s">
         <v>210</v>
       </c>
@@ -2760,7 +3051,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="42"/>
-      <c r="B104" s="29" t="s">
+      <c r="B104" s="32" t="s">
         <v>217</v>
       </c>
       <c r="C104" s="23" t="s">
@@ -2772,7 +3063,7 @@
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="42"/>
-      <c r="B105" s="35"/>
+      <c r="B105" s="33"/>
       <c r="C105" s="11" t="s">
         <v>221</v>
       </c>
@@ -2782,7 +3073,7 @@
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="42"/>
-      <c r="B106" s="29" t="s">
+      <c r="B106" s="32" t="s">
         <v>222</v>
       </c>
       <c r="C106" s="23" t="s">
@@ -2794,7 +3085,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="42"/>
-      <c r="B107" s="30"/>
+      <c r="B107" s="34"/>
       <c r="C107" s="9" t="s">
         <v>233</v>
       </c>
@@ -2804,7 +3095,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="42"/>
-      <c r="B108" s="30"/>
+      <c r="B108" s="34"/>
       <c r="C108" s="20" t="s">
         <v>234</v>
       </c>
@@ -2814,7 +3105,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="42"/>
-      <c r="B109" s="30"/>
+      <c r="B109" s="34"/>
       <c r="C109" s="9" t="s">
         <v>235</v>
       </c>
@@ -2824,7 +3115,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="42"/>
-      <c r="B110" s="30"/>
+      <c r="B110" s="34"/>
       <c r="C110" s="20" t="s">
         <v>236</v>
       </c>
@@ -2834,7 +3125,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="42"/>
-      <c r="B111" s="30"/>
+      <c r="B111" s="34"/>
       <c r="C111" s="9" t="s">
         <v>237</v>
       </c>
@@ -2844,7 +3135,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="42"/>
-      <c r="B112" s="30"/>
+      <c r="B112" s="34"/>
       <c r="C112" s="20" t="s">
         <v>238</v>
       </c>
@@ -2854,7 +3145,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="42"/>
-      <c r="B113" s="30"/>
+      <c r="B113" s="34"/>
       <c r="C113" s="9" t="s">
         <v>239</v>
       </c>
@@ -2864,7 +3155,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="42"/>
-      <c r="B114" s="30"/>
+      <c r="B114" s="34"/>
       <c r="C114" s="20" t="s">
         <v>240</v>
       </c>
@@ -2874,7 +3165,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="42"/>
-      <c r="B115" s="30"/>
+      <c r="B115" s="34"/>
       <c r="C115" s="9" t="s">
         <v>241</v>
       </c>
@@ -2884,7 +3175,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="42"/>
-      <c r="B116" s="30"/>
+      <c r="B116" s="34"/>
       <c r="C116" s="20" t="s">
         <v>242</v>
       </c>
@@ -2894,7 +3185,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="42"/>
-      <c r="B117" s="30"/>
+      <c r="B117" s="34"/>
       <c r="C117" s="9" t="s">
         <v>243</v>
       </c>
@@ -2904,7 +3195,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="42"/>
-      <c r="B118" s="30"/>
+      <c r="B118" s="34"/>
       <c r="C118" s="20" t="s">
         <v>244</v>
       </c>
@@ -2914,7 +3205,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="42"/>
-      <c r="B119" s="30"/>
+      <c r="B119" s="34"/>
       <c r="C119" s="9" t="s">
         <v>245</v>
       </c>
@@ -2924,7 +3215,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="42"/>
-      <c r="B120" s="30"/>
+      <c r="B120" s="34"/>
       <c r="C120" s="20" t="s">
         <v>246</v>
       </c>
@@ -2934,7 +3225,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="42"/>
-      <c r="B121" s="30"/>
+      <c r="B121" s="34"/>
       <c r="C121" s="9" t="s">
         <v>247</v>
       </c>
@@ -2944,7 +3235,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="42"/>
-      <c r="B122" s="30"/>
+      <c r="B122" s="34"/>
       <c r="C122" s="20" t="s">
         <v>248</v>
       </c>
@@ -2954,7 +3245,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="42"/>
-      <c r="B123" s="30"/>
+      <c r="B123" s="34"/>
       <c r="C123" s="9" t="s">
         <v>277</v>
       </c>
@@ -2964,7 +3255,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="42"/>
-      <c r="B124" s="30"/>
+      <c r="B124" s="34"/>
       <c r="C124" s="20" t="s">
         <v>278</v>
       </c>
@@ -2974,7 +3265,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="42"/>
-      <c r="B125" s="30"/>
+      <c r="B125" s="34"/>
       <c r="C125" s="9" t="s">
         <v>279</v>
       </c>
@@ -2984,7 +3275,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="42"/>
-      <c r="B126" s="30"/>
+      <c r="B126" s="34"/>
       <c r="C126" s="20" t="s">
         <v>280</v>
       </c>
@@ -2994,7 +3285,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="42"/>
-      <c r="B127" s="30"/>
+      <c r="B127" s="34"/>
       <c r="C127" s="9" t="s">
         <v>281</v>
       </c>
@@ -3004,7 +3295,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="42"/>
-      <c r="B128" s="30"/>
+      <c r="B128" s="34"/>
       <c r="C128" s="20" t="s">
         <v>282</v>
       </c>
@@ -3014,7 +3305,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="42"/>
-      <c r="B129" s="30"/>
+      <c r="B129" s="34"/>
       <c r="C129" s="9" t="s">
         <v>283</v>
       </c>
@@ -3024,7 +3315,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="42"/>
-      <c r="B130" s="30"/>
+      <c r="B130" s="34"/>
       <c r="C130" s="20" t="s">
         <v>284</v>
       </c>
@@ -3034,7 +3325,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="42"/>
-      <c r="B131" s="30"/>
+      <c r="B131" s="34"/>
       <c r="C131" s="9" t="s">
         <v>285</v>
       </c>
@@ -3044,7 +3335,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="42"/>
-      <c r="B132" s="30"/>
+      <c r="B132" s="34"/>
       <c r="C132" s="20" t="s">
         <v>286</v>
       </c>
@@ -3054,7 +3345,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="42"/>
-      <c r="B133" s="30"/>
+      <c r="B133" s="34"/>
       <c r="C133" s="9" t="s">
         <v>287</v>
       </c>
@@ -3064,7 +3355,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="42"/>
-      <c r="B134" s="30"/>
+      <c r="B134" s="34"/>
       <c r="C134" s="20" t="s">
         <v>288</v>
       </c>
@@ -3074,7 +3365,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="42"/>
-      <c r="B135" s="30"/>
+      <c r="B135" s="34"/>
       <c r="C135" s="9" t="s">
         <v>289</v>
       </c>
@@ -3084,7 +3375,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="42"/>
-      <c r="B136" s="30"/>
+      <c r="B136" s="34"/>
       <c r="C136" s="20" t="s">
         <v>290</v>
       </c>
@@ -3094,7 +3385,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="42"/>
-      <c r="B137" s="30"/>
+      <c r="B137" s="34"/>
       <c r="C137" s="9" t="s">
         <v>291</v>
       </c>
@@ -3104,7 +3395,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="42"/>
-      <c r="B138" s="30"/>
+      <c r="B138" s="34"/>
       <c r="C138" s="20" t="s">
         <v>292</v>
       </c>
@@ -3114,7 +3405,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="42"/>
-      <c r="B139" s="30"/>
+      <c r="B139" s="34"/>
       <c r="C139" s="9" t="s">
         <v>293</v>
       </c>
@@ -3124,7 +3415,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="42"/>
-      <c r="B140" s="30"/>
+      <c r="B140" s="34"/>
       <c r="C140" s="20" t="s">
         <v>294</v>
       </c>
@@ -3134,7 +3425,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="42"/>
-      <c r="B141" s="30"/>
+      <c r="B141" s="34"/>
       <c r="C141" s="9" t="s">
         <v>295</v>
       </c>
@@ -3144,7 +3435,7 @@
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="42"/>
-      <c r="B142" s="35"/>
+      <c r="B142" s="33"/>
       <c r="C142" s="28" t="s">
         <v>296</v>
       </c>
@@ -3154,7 +3445,7 @@
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="42"/>
-      <c r="B143" s="29" t="s">
+      <c r="B143" s="32" t="s">
         <v>297</v>
       </c>
       <c r="C143" s="21" t="s">
@@ -3166,7 +3457,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="42"/>
-      <c r="B144" s="30"/>
+      <c r="B144" s="34"/>
       <c r="C144" s="20" t="s">
         <v>299</v>
       </c>
@@ -3176,7 +3467,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="42"/>
-      <c r="B145" s="30"/>
+      <c r="B145" s="34"/>
       <c r="C145" s="9" t="s">
         <v>300</v>
       </c>
@@ -3186,7 +3477,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="42"/>
-      <c r="B146" s="30"/>
+      <c r="B146" s="34"/>
       <c r="C146" s="20" t="s">
         <v>301</v>
       </c>
@@ -3196,7 +3487,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="42"/>
-      <c r="B147" s="30"/>
+      <c r="B147" s="34"/>
       <c r="C147" s="9" t="s">
         <v>307</v>
       </c>
@@ -3206,7 +3497,7 @@
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="42"/>
-      <c r="B148" s="31"/>
+      <c r="B148" s="40"/>
       <c r="C148" s="25" t="s">
         <v>308</v>
       </c>
@@ -3216,19 +3507,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B91:B101"/>
-    <mergeCell ref="B82:B90"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="B106:B142"/>
+    <mergeCell ref="B143:B148"/>
+    <mergeCell ref="A2:A148"/>
     <mergeCell ref="B60:B63"/>
     <mergeCell ref="B64:B81"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="B50:B54"/>
     <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B143:B148"/>
-    <mergeCell ref="A2:A148"/>
+    <mergeCell ref="B91:B101"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="B106:B142"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3238,12 +3529,471 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EFE84B-6178-4324-9A94-999BE39EC719}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="200.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>352</v>
+      </c>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>373</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>321</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>322</v>
+      </c>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>349</v>
+      </c>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="45" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D29" s="49" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="54"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A38"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B22:B38"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[CAN2-23] Removed mention of the unused PROP state
</commit_message>
<xml_diff>
--- a/CAN_Controller_Design_Specifications_Andrew.xlsx
+++ b/CAN_Controller_Design_Specifications_Andrew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7FE65D-8214-409A-85CB-68D80F943F0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC5FBEB-6495-4D74-81D1-6695BCC6E48E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bit Stream Processor" sheetId="1" r:id="rId1"/>
@@ -1141,9 +1141,6 @@
     <t>The Module shall set int_rx_prev_compare equal to int_rx_compare on a rising edge of can_clk.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Module shall set int_state_next to TS1 when int_state is either SYNC or PROP and int_state_counter is less than int_ts1. </t>
-  </si>
-  <si>
     <t>The Module shall initialize int_ts2 equal to i_ts2 + 1 on system startup.</t>
   </si>
   <si>
@@ -1190,6 +1187,9 @@
   </si>
   <si>
     <t xml:space="preserve">The Module shall set int_state_next to TS2 when int_state_counter is less than int_ts1 + int_ts2 and greater than or equal to int_ts1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Module shall set int_state_next to TS1 when int_state is either SYNC and int_state_counter is less than int_ts1. </t>
   </si>
 </sst>
 </file>
@@ -3531,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EFE84B-6178-4324-9A94-999BE39EC719}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,7 +3628,7 @@
         <v>359</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
@@ -3643,7 +3643,7 @@
         <v>360</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="41"/>
@@ -3735,7 +3735,7 @@
         <v>361</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3745,7 +3745,7 @@
         <v>362</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3787,7 +3787,7 @@
         <v>330</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>371</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>331</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3899,7 +3899,7 @@
         <v>363</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>364</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3919,7 +3919,7 @@
         <v>365</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,7 +3929,7 @@
         <v>366</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
         <v>367</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,7 +3949,7 @@
         <v>368</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,27 +3959,27 @@
         <v>369</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="51"/>
       <c r="C37" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="56"/>
       <c r="B38" s="57"/>
       <c r="C38" s="36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>